<commit_message>
Initial commit: bootstrap cargomen (copied from iwealth)
</commit_message>
<xml_diff>
--- a/files/Karurvyasya_statements.xlsx
+++ b/files/Karurvyasya_statements.xlsx
@@ -546,8 +546,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="56" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="56" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
@@ -557,14 +557,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sr_no</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>sr_no</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>As on 31.03.2025</t>
@@ -587,12 +587,12 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Capital</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr"/>
       <c r="C2" s="3" t="n">
         <v>16102</v>
       </c>
@@ -603,12 +603,12 @@
       <c r="F2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr"/>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Reserves and surplus</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr"/>
       <c r="C3" s="3" t="n">
         <v>1176852</v>
       </c>
@@ -619,12 +619,12 @@
       <c r="F3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr"/>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Deposits</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr"/>
       <c r="C4" s="3" t="n">
         <v>10207799</v>
       </c>
@@ -635,12 +635,12 @@
       <c r="F4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr"/>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>Borrowings</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr"/>
       <c r="C5" s="3" t="n">
         <v>121698</v>
       </c>
@@ -651,12 +651,12 @@
       <c r="F5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr"/>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Other liabilities and provisions</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr"/>
       <c r="C6" s="3" t="n">
         <v>414291</v>
       </c>
@@ -667,12 +667,12 @@
       <c r="F6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr"/>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr"/>
       <c r="C7" s="3" t="n">
         <v>11936742</v>
       </c>
@@ -683,12 +683,12 @@
       <c r="F7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr"/>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Cash &amp; balances with Reserve Bank of India</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr"/>
       <c r="C8" s="3" t="n">
         <v>735419</v>
       </c>
@@ -699,12 +699,12 @@
       <c r="F8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr"/>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Balances with banks and money at call and short notice</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr"/>
       <c r="C9" s="3" t="n">
         <v>45253</v>
       </c>
@@ -715,12 +715,12 @@
       <c r="F9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr"/>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Investments</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr"/>
       <c r="C10" s="3" t="n">
         <v>2383125</v>
       </c>
@@ -731,12 +731,12 @@
       <c r="F10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>Advances</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="3" t="n">
         <v>8400454</v>
       </c>
@@ -747,12 +747,12 @@
       <c r="F11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr"/>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Fixed assets</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="3" t="n">
         <v>49017</v>
       </c>
@@ -763,12 +763,12 @@
       <c r="F12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr"/>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Other assets</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="3" t="n">
         <v>323474</v>
       </c>
@@ -779,12 +779,12 @@
       <c r="F13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr"/>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr"/>
       <c r="C14" s="3" t="n">
         <v>11936742</v>
       </c>
@@ -805,7 +805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -814,8 +814,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
     <col width="26" customWidth="1" min="3" max="3"/>
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -826,14 +826,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sr_no</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>sr_no</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Quarter ended 31-03-2025</t>
@@ -861,12 +861,12 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>a) Interest / discount on advances / bills</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="n">
         <v>208045</v>
       </c>
@@ -884,12 +884,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr"/>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>b) Income on investments</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="n">
         <v>42140</v>
       </c>
@@ -907,12 +907,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr"/>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>c) Interest on balances with Reserve Bank of India &amp; other interbank funds</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
       <c r="C4" s="3" t="n">
         <v>982</v>
       </c>
@@ -930,12 +930,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr"/>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>d) Other interest</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
       <c r="C5" s="3" t="n">
         <v>426</v>
       </c>
@@ -953,13 +953,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Interest earned (a+b+c+d)</t>
         </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>1</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>251593</v>
@@ -978,13 +978,13 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Other income</t>
         </is>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>2</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>50933</v>
@@ -1003,13 +1003,13 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Total income (1+2)</t>
         </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>3</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>302526</v>
@@ -1028,13 +1028,13 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Interest expended</t>
         </is>
-      </c>
-      <c r="B9" s="3" t="n">
-        <v>4</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>142667</v>
@@ -1053,12 +1053,12 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr"/>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>(i) Employees cost</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr"/>
       <c r="C10" s="3" t="n">
         <v>38493</v>
       </c>
@@ -1076,12 +1076,12 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>(ii) Other operating expenses</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr"/>
       <c r="C11" s="3" t="n">
         <v>37869</v>
       </c>
@@ -1099,13 +1099,13 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Operating expenses (i+ii)</t>
         </is>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>5</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>76362</v>
@@ -1124,13 +1124,13 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Total expenditure (excluding provisions and contingencies) (4+5)</t>
         </is>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>6</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>219029</v>
@@ -1149,13 +1149,13 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Operating profit before provisions and contingencies (3-6)</t>
         </is>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>7</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>83497</v>
@@ -1174,13 +1174,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>Provisions (other than tax) and contingencies</t>
         </is>
-      </c>
-      <c r="B15" s="3" t="n">
-        <v>8</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>16140</v>
@@ -1199,13 +1199,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>Exceptional items</t>
         </is>
-      </c>
-      <c r="B16" s="3" t="n">
-        <v>9</v>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
       <c r="D16" s="3" t="inlineStr"/>
@@ -1214,13 +1214,13 @@
       <c r="G16" s="3" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Profit from ordinary activities before tax (7-8-9)</t>
         </is>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>10</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>67357</v>
@@ -1239,13 +1239,13 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="inlineStr">
+      <c r="A18" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>Tax expense</t>
         </is>
-      </c>
-      <c r="B18" s="3" t="n">
-        <v>11</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>16021</v>
@@ -1264,13 +1264,13 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+      <c r="A19" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>Net profit from ordinary activities after tax (10-11)</t>
         </is>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>12</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>51336</v>
@@ -1289,13 +1289,13 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="A20" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>Extraordinary items (net of tax expense)</t>
         </is>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>13</v>
       </c>
       <c r="C20" s="3" t="inlineStr"/>
       <c r="D20" s="3" t="inlineStr"/>
@@ -1304,13 +1304,13 @@
       <c r="G20" s="3" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="inlineStr">
+      <c r="A21" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>Net profit for the period (12-13)</t>
         </is>
-      </c>
-      <c r="B21" s="3" t="n">
-        <v>14</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>51336</v>
@@ -1329,13 +1329,13 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="inlineStr">
+      <c r="A22" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>Paid-up equity share capital (FV Rs.2/- per share)</t>
         </is>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>15</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>16102</v>
@@ -1354,13 +1354,13 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+      <c r="A23" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Reserves excluding revaluation reserve</t>
         </is>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>16</v>
       </c>
       <c r="C23" s="3" t="inlineStr"/>
       <c r="D23" s="3" t="inlineStr"/>
@@ -1373,19 +1373,345 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>Analytical ratio</t>
-        </is>
-      </c>
-      <c r="B24" s="3" t="n">
-        <v>17</v>
+      <c r="A24" s="3" t="inlineStr"/>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>(i) % of shares held by Government of India</t>
+        </is>
       </c>
       <c r="C24" s="3" t="inlineStr"/>
       <c r="D24" s="3" t="inlineStr"/>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3" t="inlineStr"/>
       <c r="G24" s="3" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr"/>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>(ii) Capital adequacy ratio - Basel III (%)</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>18.17</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>16.67</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>18.17</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>16.67</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr"/>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>a) Basic EPS before and after extraordinary items</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>24.13</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>19.99</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr"/>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>b) Diluted EPS before and after extraordinary items</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>6.37</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>24.12</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>19.97</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr"/>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>(iii) Earnings per share (EPS) (Rs.)</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr"/>
+      <c r="D28" s="3" t="inlineStr"/>
+      <c r="E28" s="3" t="inlineStr"/>
+      <c r="F28" s="3" t="inlineStr"/>
+      <c r="G28" s="3" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr"/>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>a) Gross NPA</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>64180</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>69092</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>104164</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>64180</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>104164</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr"/>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>b) Net NPA</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>16621</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>16669</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>29797</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>16621</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>29797</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr"/>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>c) % of Gross NPA</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr"/>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>d) % of Net NPA</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr"/>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>(iv) NPA ratios</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr"/>
+      <c r="D33" s="3" t="inlineStr"/>
+      <c r="E33" s="3" t="inlineStr"/>
+      <c r="F33" s="3" t="inlineStr"/>
+      <c r="G33" s="3" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr"/>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>(v) Return on asset (annualised) (%)</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="G34" s="3" t="n">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>Analytical ratio</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr"/>
+      <c r="D35" s="3" t="inlineStr"/>
+      <c r="E35" s="3" t="inlineStr"/>
+      <c r="F35" s="3" t="inlineStr"/>
+      <c r="G35" s="3" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Net worth²</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>1164488</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>1131433</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>980282</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>1164488</v>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>980282</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>Paid up debt capital/ Outstanding debt³ (%)</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr"/>
+      <c r="D37" s="3" t="inlineStr"/>
+      <c r="E37" s="3" t="inlineStr"/>
+      <c r="F37" s="3" t="inlineStr"/>
+      <c r="G37" s="3" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Debt/equity ratio</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Total debts to total assets (%)</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr"/>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Analytical Ratios and other disclosures</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr"/>
+      <c r="D40" s="3" t="inlineStr"/>
+      <c r="E40" s="3" t="inlineStr"/>
+      <c r="F40" s="3" t="inlineStr"/>
+      <c r="G40" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1398,7 +1724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1407,25 +1733,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sr_no</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>sr_no</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Year ended 31-03-2025</t>
@@ -1436,25 +1760,13 @@
           <t>Year ended 31-03-2024</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>c3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>c4</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Net Profit as per Profit and Loss account</t>
         </is>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1.1</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>194164</v>
@@ -1462,233 +1774,199 @@
       <c r="D2" s="3" t="n">
         <v>160481</v>
       </c>
-      <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr"/>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Adjustments for</t>
         </is>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>1.2</v>
       </c>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="2" t="inlineStr"/>
-      <c r="F3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr"/>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Depreciation on Bank's property</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
       <c r="C4" s="3" t="n">
         <v>11373</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>10026</v>
       </c>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr"/>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>Interest paid on TIER II bonds</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
       <c r="C5" s="3" t="n">
         <v>5501</v>
       </c>
       <c r="D5" s="3" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr"/>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Provisions for other contingencies</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
       <c r="C6" s="3" t="n">
         <v>11785</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>10842</v>
       </c>
-      <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr"/>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Provision for taxes</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr"/>
       <c r="C7" s="3" t="n">
         <v>64909</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>49538</v>
       </c>
-      <c r="E7" s="2" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr"/>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Provision for depreciation on investment</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr"/>
       <c r="C8" s="3" t="inlineStr"/>
       <c r="D8" s="3" t="n">
         <v>-25461</v>
       </c>
-      <c r="E8" s="2" t="inlineStr"/>
-      <c r="F8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr"/>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Provision for standard assets</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr"/>
       <c r="C9" s="3" t="n">
         <v>3995</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>4474</v>
       </c>
-      <c r="E9" s="2" t="inlineStr"/>
-      <c r="F9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr"/>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Provision for bad and doubtful debts</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr"/>
       <c r="C10" s="3" t="n">
         <v>44040</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>42766</v>
       </c>
-      <c r="E10" s="2" t="inlineStr"/>
-      <c r="F10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>Provision for non performing investments</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr"/>
       <c r="C11" s="3" t="n">
         <v>2340</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>14813</v>
       </c>
-      <c r="E11" s="2" t="inlineStr"/>
-      <c r="F11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr"/>
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Provision for compensation absences</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr"/>
       <c r="C12" s="3" t="n">
         <v>3130</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>7264</v>
       </c>
-      <c r="E12" s="2" t="inlineStr"/>
-      <c r="F12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr"/>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Provision for medical leave</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr"/>
       <c r="C13" s="3" t="n">
         <v>1124</v>
       </c>
       <c r="D13" s="3" t="inlineStr"/>
-      <c r="E13" s="2" t="inlineStr"/>
-      <c r="F13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr"/>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Amortization of premium paid on Held to Maturity (HTM) investments</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr"/>
       <c r="C14" s="3" t="n">
         <v>8528</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>10362</v>
       </c>
-      <c r="E14" s="2" t="inlineStr"/>
-      <c r="F14" s="2" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr"/>
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>Provision for employees stock option plan / scheme</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr"/>
       <c r="C15" s="3" t="n">
         <v>275</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>341</v>
       </c>
-      <c r="E15" s="2" t="inlineStr"/>
-      <c r="F15" s="2" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr"/>
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>(Profit)/Loss on sale of fixed assets (net)</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr"/>
       <c r="C16" s="3" t="n">
         <v>-306</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>-783</v>
       </c>
-      <c r="E16" s="2" t="inlineStr"/>
-      <c r="F16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr"/>
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Operating profit before working capital changes</t>
         </is>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>1.3</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>345357</v>
@@ -1696,163 +1974,135 @@
       <c r="D17" s="3" t="n">
         <v>290164</v>
       </c>
-      <c r="E17" s="2" t="inlineStr"/>
-      <c r="F17" s="2" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr"/>
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>Adjustments for working capital changes</t>
         </is>
-      </c>
-      <c r="B18" s="3" t="n">
-        <v>1.4</v>
       </c>
       <c r="C18" s="3" t="inlineStr"/>
       <c r="D18" s="3" t="inlineStr"/>
-      <c r="E18" s="2" t="inlineStr"/>
-      <c r="F18" s="2" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr"/>
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>(Increase)/Decrease in investments (excluding HTM investments)</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr"/>
       <c r="C19" s="3" t="n">
         <v>52251</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>-232613</v>
       </c>
-      <c r="E19" s="2" t="inlineStr"/>
-      <c r="F19" s="2" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr"/>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>(Increase) / Decrease in advances</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr"/>
       <c r="C20" s="3" t="n">
         <v>-1077642</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>-1095896</v>
       </c>
-      <c r="E20" s="2" t="inlineStr"/>
-      <c r="F20" s="2" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr"/>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>(Increase)/Decrease in other assets</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr"/>
       <c r="C21" s="3" t="n">
         <v>8812</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>-40565</v>
       </c>
-      <c r="E21" s="2" t="inlineStr"/>
-      <c r="F21" s="2" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr"/>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>Increase (Decrease) in deposits</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr"/>
       <c r="C22" s="3" t="n">
         <v>1296526</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>1247514</v>
       </c>
-      <c r="E22" s="2" t="inlineStr"/>
-      <c r="F22" s="2" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr"/>
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Increase/(Decrease) in borrowings</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr"/>
       <c r="C23" s="3" t="n">
         <v>-126137</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>153333</v>
       </c>
-      <c r="E23" s="2" t="inlineStr"/>
-      <c r="F23" s="2" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr"/>
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>Increase/(Decrease) in other liabilities and provisions</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr"/>
       <c r="C24" s="3" t="n">
         <v>1039</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>18969</v>
       </c>
-      <c r="E24" s="2" t="inlineStr"/>
-      <c r="F24" s="2" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Operating profit after working capital changes</t>
-        </is>
-      </c>
-      <c r="B25" s="3" t="n">
-        <v>1.5</v>
+      <c r="A25" s="2" t="inlineStr"/>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>Direct taxes paid</t>
+        </is>
       </c>
       <c r="C25" s="3" t="n">
-        <v>500206</v>
+        <v>-51500</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>340906</v>
-      </c>
-      <c r="E25" s="2" t="inlineStr"/>
-      <c r="F25" s="2" t="inlineStr"/>
+        <v>-45500</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Direct taxes paid</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>1.6</v>
+      <c r="A26" s="2" t="inlineStr"/>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>Net cash flow (from)/ used in operating activities</t>
+        </is>
       </c>
       <c r="C26" s="3" t="n">
-        <v>-51500</v>
+        <v>448706</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>-45500</v>
-      </c>
-      <c r="E26" s="2" t="inlineStr"/>
-      <c r="F26" s="2" t="inlineStr"/>
+        <v>295406</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>Net cash flow (from)/ used in operating activities</t>
-        </is>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>1.7</v>
+      <c r="A27" s="2" t="inlineStr"/>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>Cash flow from/(used in) operating activities</t>
+        </is>
       </c>
       <c r="C27" s="3" t="n">
         <v>448706</v>
@@ -1860,89 +2110,69 @@
       <c r="D27" s="3" t="n">
         <v>295406</v>
       </c>
-      <c r="E27" s="2" t="inlineStr"/>
-      <c r="F27" s="2" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Cash flow from/(used in) operating activities</t>
-        </is>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>1</v>
+      <c r="A28" s="2" t="inlineStr"/>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>Purchase of fixed assets</t>
+        </is>
       </c>
       <c r="C28" s="3" t="n">
-        <v>448706</v>
+        <v>-17163</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>295406</v>
-      </c>
-      <c r="E28" s="2" t="inlineStr"/>
-      <c r="F28" s="2" t="inlineStr"/>
+        <v>-9810</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Purchase of fixed assets</t>
-        </is>
-      </c>
-      <c r="B29" s="3" t="n">
-        <v>2.1</v>
+      <c r="A29" s="2" t="inlineStr"/>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>(Increase)/Decrease in HTM investments</t>
+        </is>
       </c>
       <c r="C29" s="3" t="n">
-        <v>-17163</v>
+        <v>-198283</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>-9810</v>
-      </c>
-      <c r="E29" s="2" t="inlineStr"/>
-      <c r="F29" s="2" t="inlineStr"/>
+        <v>-120621</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>(Increase)/Decrease in HTM investments</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="n">
-        <v>2.2</v>
+      <c r="A30" s="2" t="inlineStr"/>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>Sale of fixed assets / other assets</t>
+        </is>
       </c>
       <c r="C30" s="3" t="n">
-        <v>-198283</v>
+        <v>366</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>-120621</v>
-      </c>
-      <c r="E30" s="2" t="inlineStr"/>
-      <c r="F30" s="2" t="inlineStr"/>
+        <v>783</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Sale of fixed assets / other assets</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>2.3</v>
+      <c r="A31" s="2" t="inlineStr"/>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>Net cash flow from/ (used in) investing activities</t>
+        </is>
       </c>
       <c r="C31" s="3" t="n">
-        <v>366</v>
+        <v>-215080</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>783</v>
-      </c>
-      <c r="E31" s="2" t="inlineStr"/>
-      <c r="F31" s="2" t="inlineStr"/>
+        <v>-129648</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Net cash flow from/ (used in) investing activities</t>
-        </is>
-      </c>
-      <c r="B32" s="3" t="n">
-        <v>2.4</v>
+      <c r="A32" s="2" t="inlineStr"/>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Cash flow from investing activities</t>
+        </is>
       </c>
       <c r="C32" s="3" t="n">
         <v>-215080</v>
@@ -1950,123 +2180,93 @@
       <c r="D32" s="3" t="n">
         <v>-129648</v>
       </c>
-      <c r="E32" s="2" t="inlineStr"/>
-      <c r="F32" s="2" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Cash flow from investing activities</t>
-        </is>
-      </c>
-      <c r="B33" s="3" t="n">
-        <v>2</v>
+      <c r="A33" s="2" t="inlineStr"/>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>Proceeds from share capital</t>
+        </is>
       </c>
       <c r="C33" s="3" t="n">
-        <v>-215080</v>
+        <v>15</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>-129648</v>
-      </c>
-      <c r="E33" s="2" t="inlineStr"/>
-      <c r="F33" s="2" t="inlineStr"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Proceeds from share capital</t>
-        </is>
-      </c>
-      <c r="B34" s="3" t="n">
-        <v>3.1</v>
+      <c r="A34" s="2" t="inlineStr"/>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Proceeds from share premium</t>
+        </is>
       </c>
       <c r="C34" s="3" t="n">
-        <v>15</v>
+        <v>427</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>46</v>
-      </c>
-      <c r="E34" s="2" t="inlineStr"/>
-      <c r="F34" s="2" t="inlineStr"/>
+        <v>785</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Proceeds from share premium</t>
-        </is>
-      </c>
-      <c r="B35" s="3" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="C35" s="3" t="n">
-        <v>427</v>
-      </c>
+      <c r="A35" s="2" t="inlineStr"/>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>Increase/(Decrease) in tier II bonds</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr"/>
       <c r="D35" s="3" t="n">
-        <v>785</v>
-      </c>
-      <c r="E35" s="2" t="inlineStr"/>
-      <c r="F35" s="2" t="inlineStr"/>
+        <v>-48700</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="inlineStr">
-        <is>
-          <t>Increase/(Decrease) in tier II bonds</t>
-        </is>
-      </c>
-      <c r="B36" s="3" t="n">
-        <v>3.3</v>
+      <c r="A36" s="2" t="inlineStr"/>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Interest paid on tier II bonds</t>
+        </is>
       </c>
       <c r="C36" s="3" t="inlineStr"/>
       <c r="D36" s="3" t="n">
-        <v>-48700</v>
-      </c>
-      <c r="E36" s="2" t="inlineStr"/>
-      <c r="F36" s="2" t="inlineStr"/>
+        <v>-5501</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>Interest paid on tier Il bonds</t>
-        </is>
-      </c>
-      <c r="B37" s="3" t="n">
-        <v>3.4</v>
+      <c r="A37" s="2" t="inlineStr"/>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>Dividend paid</t>
+        </is>
       </c>
       <c r="C37" s="3" t="n">
-        <v>-5501</v>
+        <v>-19253</v>
       </c>
       <c r="D37" s="3" t="n">
         <v>-16044</v>
       </c>
-      <c r="E37" s="2" t="inlineStr"/>
-      <c r="F37" s="2" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>Dividend paid</t>
-        </is>
-      </c>
-      <c r="B38" s="3" t="n">
-        <v>3.5</v>
+      <c r="A38" s="2" t="inlineStr"/>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Net cash flow from/ (used in) financing activities</t>
+        </is>
       </c>
       <c r="C38" s="3" t="n">
-        <v>-19253</v>
+        <v>-18811</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>-16044</v>
-      </c>
-      <c r="E38" s="2" t="inlineStr"/>
-      <c r="F38" s="2" t="inlineStr"/>
+        <v>-69414</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t>Net cash flow from/ (used in) financing activities</t>
-        </is>
-      </c>
-      <c r="B39" s="3" t="n">
-        <v>3.6</v>
+      <c r="A39" s="2" t="inlineStr"/>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Cash flow from financing activities</t>
+        </is>
       </c>
       <c r="C39" s="3" t="n">
         <v>-18811</v>
@@ -2074,80 +2274,58 @@
       <c r="D39" s="3" t="n">
         <v>-69414</v>
       </c>
-      <c r="E39" s="2" t="inlineStr"/>
-      <c r="F39" s="2" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="inlineStr">
-        <is>
-          <t>Cash flow from financing activities</t>
-        </is>
-      </c>
-      <c r="B40" s="3" t="n">
-        <v>3</v>
+      <c r="A40" s="2" t="inlineStr"/>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Net Increase/(decrease) in cash &amp; cash equivalents</t>
+        </is>
       </c>
       <c r="C40" s="3" t="n">
-        <v>-18811</v>
+        <v>214815</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>-69414</v>
-      </c>
-      <c r="E40" s="2" t="inlineStr"/>
-      <c r="F40" s="2" t="inlineStr"/>
+        <v>96344</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="inlineStr">
-        <is>
-          <t>Net Increase/(decrease) in cash &amp; cash equivalents</t>
-        </is>
-      </c>
-      <c r="B41" s="3" t="n">
-        <v>4</v>
+      <c r="A41" s="2" t="inlineStr"/>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>Cash and cash equivalents at the beginning of the year</t>
+        </is>
       </c>
       <c r="C41" s="3" t="n">
-        <v>214815</v>
+        <v>565857</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>96344</v>
-      </c>
-      <c r="E41" s="2" t="inlineStr"/>
-      <c r="F41" s="2" t="inlineStr"/>
+        <v>469513</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="inlineStr">
-        <is>
-          <t>Cash and cash equivalents at the beginning of the year</t>
-        </is>
-      </c>
-      <c r="B42" s="3" t="n">
-        <v>5</v>
+      <c r="A42" s="2" t="inlineStr"/>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>Cash and cash equivalents at the end of the year</t>
+        </is>
       </c>
       <c r="C42" s="3" t="n">
+        <v>780672</v>
+      </c>
+      <c r="D42" s="3" t="n">
         <v>565857</v>
       </c>
-      <c r="D42" s="3" t="n">
-        <v>469513</v>
-      </c>
-      <c r="E42" s="2" t="inlineStr"/>
-      <c r="F42" s="2" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>Cash and cash equivalents at the end of the year</t>
-        </is>
-      </c>
-      <c r="B43" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C43" s="3" t="n">
-        <v>780672</v>
-      </c>
-      <c r="D43" s="3" t="n">
-        <v>565857</v>
-      </c>
-      <c r="E43" s="2" t="inlineStr"/>
-      <c r="F43" s="2" t="inlineStr"/>
+      <c r="A43" s="2" t="inlineStr"/>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>Cash and Cash Equivalents Reconciliation</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr"/>
+      <c r="D43" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2324,7 +2502,7 @@
     <col width="26" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
   </cols>
@@ -2400,7 +2578,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -2433,12 +2611,12 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>Prior period</t>
+          <t>Previous period</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -2601,7 +2779,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>current fiscal year</t>
+          <t>current year</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
@@ -2643,7 +2821,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>previous fiscal year</t>
+          <t>previous year</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">

</xml_diff>